<commit_message>
new .ttl from Google sheet has been generated
</commit_message>
<xml_diff>
--- a/aspect-taxonomy.xlsx
+++ b/aspect-taxonomy.xlsx
@@ -856,7 +856,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>0.1.0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1739,19 +1739,19 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Atmospheric Terms</t>
+          <t>Enviromental Codition Terms</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>This is a category of variables, parameters, and constants associated with atmopshere.</t>
+          <t>This is a category of variables, parameters, and constants associated with enviromental coditions in which a wind power plant operates.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr"/>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -2023,7 +2023,7 @@
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -2080,7 +2080,7 @@
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -2470,7 +2470,7 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -2527,7 +2527,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -2584,7 +2584,7 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -2641,7 +2641,7 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -2698,7 +2698,7 @@
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -2755,7 +2755,7 @@
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -2812,7 +2812,7 @@
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -2865,7 +2865,7 @@
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>aspect:AtmosphericTerms</t>
+          <t>aspect:EnviromentalCoditionTerms</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">

</xml_diff>